<commit_message>
verdiep 2 reeds klaar
</commit_message>
<xml_diff>
--- a/documentation/project2Acsv_versieP.xlsx
+++ b/documentation/project2Acsv_versieP.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\KUleuven\InDoorDeviceLocalisation\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documents\school\Projectlab2\InDoorDeviceLocalisation\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1941BAEB-54C9-4551-ABDF-78B9CDE84FE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{1941BAEB-54C9-4551-ABDF-78B9CDE84FE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{3BDAE2B9-36FF-4787-BC3E-FA94165B3F0E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" activeTab="1"/>
+    <workbookView xWindow="20355" yWindow="0" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="project2Acsv_versieP" sheetId="1" r:id="rId1"/>
     <sheet name="Blad1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -806,7 +814,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1316,24 +1324,24 @@
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Berekening" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Controlecel" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Gekoppelde cel" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Goed" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Invoer" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Kop 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Kop 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Kop 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Kop 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutraal" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notitie" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ongeldig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Totaal" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uitvoer" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1349,7 +1357,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1644,25 +1652,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D62"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" customWidth="1"/>
+    <col min="4" max="4" width="60.21875" customWidth="1"/>
+    <col min="5" max="5" width="2" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1682,7 +1690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1705,7 +1713,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1728,7 +1736,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1751,7 +1759,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1774,7 +1782,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1797,7 +1805,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1820,7 +1828,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1843,7 +1851,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1863,7 +1871,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1883,7 +1891,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1903,7 +1911,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1923,7 +1931,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1946,7 +1954,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1969,7 +1977,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1992,7 +2000,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2015,7 +2023,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2038,7 +2046,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2061,7 +2069,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2084,7 +2092,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2104,7 +2112,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2124,7 +2132,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2147,7 +2155,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2170,7 +2178,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2193,7 +2201,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2216,7 +2224,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2239,7 +2247,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2262,7 +2270,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2282,7 +2290,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2305,7 +2313,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2328,7 +2336,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2351,7 +2359,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2374,7 +2382,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2397,7 +2405,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2420,7 +2428,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2443,7 +2451,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2466,7 +2474,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2489,7 +2497,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2509,7 +2517,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2532,7 +2540,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2555,7 +2563,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2578,7 +2586,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2601,7 +2609,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2624,7 +2632,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2647,7 +2655,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2670,7 +2678,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2693,7 +2701,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2716,7 +2724,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2739,7 +2747,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2762,7 +2770,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2785,7 +2793,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2808,7 +2816,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2831,7 +2839,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2854,7 +2862,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2877,7 +2885,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2900,7 +2908,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2923,7 +2931,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2946,7 +2954,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2969,7 +2977,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2992,7 +3000,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3015,7 +3023,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3041,7 +3049,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3064,7 +3072,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>219</v>
       </c>
@@ -3081,7 +3089,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>223</v>
       </c>
@@ -3098,7 +3106,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>226</v>
       </c>
@@ -3115,7 +3123,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>229</v>
       </c>
@@ -3139,21 +3147,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:L11"/>
+    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>232</v>
       </c>
@@ -3165,7 +3173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>233</v>
       </c>
@@ -3177,7 +3185,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>234</v>
       </c>
@@ -3189,7 +3197,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>235</v>
       </c>
@@ -3201,7 +3209,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>236</v>
       </c>
@@ -3213,7 +3221,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>237</v>
       </c>
@@ -3225,7 +3233,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>238</v>
       </c>
@@ -3237,7 +3245,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>242</v>
       </c>
@@ -3249,7 +3257,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>245</v>
       </c>
@@ -3261,7 +3269,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>248</v>
       </c>
@@ -3273,7 +3281,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>258</v>
       </c>
@@ -3285,7 +3293,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>100</v>
       </c>
@@ -3297,7 +3305,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>101</v>
       </c>
@@ -3309,7 +3317,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>102</v>
       </c>
@@ -3321,7 +3329,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>103</v>
       </c>
@@ -3333,7 +3341,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>104</v>
       </c>
@@ -3345,7 +3353,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>105</v>
       </c>
@@ -3357,7 +3365,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>106</v>
       </c>
@@ -3369,7 +3377,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>107</v>
       </c>
@@ -3381,7 +3389,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>108</v>
       </c>
@@ -3393,7 +3401,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>200</v>
       </c>
@@ -3405,7 +3413,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>201</v>
       </c>
@@ -3417,7 +3425,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>202</v>
       </c>
@@ -3429,7 +3437,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>203</v>
       </c>
@@ -3441,7 +3449,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>204</v>
       </c>
@@ -3453,7 +3461,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>205</v>
       </c>
@@ -3465,7 +3473,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>206</v>
       </c>
@@ -3477,7 +3485,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>300</v>
       </c>
@@ -3489,7 +3497,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>301</v>
       </c>
@@ -3501,7 +3509,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>302</v>
       </c>
@@ -3513,7 +3521,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>303</v>
       </c>
@@ -3525,7 +3533,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>304</v>
       </c>
@@ -3537,7 +3545,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>305</v>
       </c>
@@ -3549,7 +3557,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>306</v>
       </c>
@@ -3561,7 +3569,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>307</v>
       </c>
@@ -3573,7 +3581,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>308</v>
       </c>
@@ -3585,7 +3593,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>309</v>
       </c>
@@ -3597,7 +3605,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>400</v>
       </c>
@@ -3609,7 +3617,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>401</v>
       </c>
@@ -3621,7 +3629,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>402</v>
       </c>
@@ -3633,7 +3641,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>403</v>
       </c>
@@ -3645,7 +3653,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>404</v>
       </c>
@@ -3657,7 +3665,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>405</v>
       </c>
@@ -3669,7 +3677,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>406</v>
       </c>
@@ -3681,7 +3689,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>407</v>
       </c>
@@ -3693,7 +3701,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>408</v>
       </c>
@@ -3705,7 +3713,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>500</v>
       </c>
@@ -3717,7 +3725,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>501</v>
       </c>
@@ -3729,7 +3737,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>502</v>
       </c>
@@ -3741,7 +3749,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>503</v>
       </c>
@@ -3753,7 +3761,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>504</v>
       </c>
@@ -3765,7 +3773,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>506</v>
       </c>
@@ -3777,7 +3785,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>507</v>
       </c>
@@ -3789,7 +3797,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>508</v>
       </c>
@@ -3801,7 +3809,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>600</v>
       </c>
@@ -3813,7 +3821,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>601</v>
       </c>
@@ -3825,7 +3833,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>602</v>
       </c>
@@ -3837,7 +3845,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>603</v>
       </c>
@@ -3849,7 +3857,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>604</v>
       </c>
@@ -3861,7 +3869,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>605</v>
       </c>
@@ -3873,7 +3881,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>606</v>
       </c>

</xml_diff>